<commit_message>
Final Push -> Includes Coursework
</commit_message>
<xml_diff>
--- a/CW/ES CW GANNT CHART.xlsx
+++ b/CW/ES CW GANNT CHART.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunet-my.sharepoint.com/personal/ld0812_lunet_lboro_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunet-my.sharepoint.com/personal/ld0812_lunet_lboro_ac_uk/Documents/Programming/ES Y1S1/Embedded-Systems-Labs-1/CW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{5187BFB9-98DC-43D1-97EE-B9DD657DAA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E13F13EC-0A96-4FF5-8EF7-2E3A4022B444}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{5187BFB9-98DC-43D1-97EE-B9DD657DAA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FDC1FC4-1C7B-403E-9E10-88BC48A20ACA}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{4411009A-E4CD-401B-92A0-59F3794AA128}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4411009A-E4CD-401B-92A0-59F3794AA128}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -693,119 +693,119 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,6 +827,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1175,505 +1179,508 @@
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="38" t="s">
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="42"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="42"/>
-      <c r="L4" s="45"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="16"/>
+      <c r="L4" s="19"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="42" t="s">
+      <c r="B5" s="50"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="16" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="42"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="16"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="42" t="s">
+      <c r="B7" s="54"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="42"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="42"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="42"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="42" t="s">
+      <c r="A12" s="45"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="16" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="42"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="42"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="42"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="16"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="42"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="16"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="42"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="16"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="42"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="16"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="42"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="16"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="42"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="16"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="42"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="16"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="42"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="16"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="42"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="16"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="42"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="16"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="42"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="16"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="16"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="42"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="16"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="42"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="16"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="42"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="16"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="42"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="16"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="42"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="16"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="42"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="16"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="29"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="42"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="16"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="42"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="16"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="31"/>
+      <c r="B36" s="11"/>
       <c r="C36" t="s">
         <v>14</v>
       </c>
-      <c r="J36" s="41"/>
+      <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="31"/>
+      <c r="B37" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
@@ -1686,23 +1693,21 @@
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="90" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>